<commit_message>
Julkaistu tehtävän palautuksen yhteydessä
</commit_message>
<xml_diff>
--- a/CNC_data.xlsx
+++ b/CNC_data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuas365-my.sharepoint.com/personal/tuomas_m_mikkola_edu_turkuamk_fi/Documents/Tutkimus- ja kehittämismenetelmät/CNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{FA12262A-488B-4907-8A1D-562E1E59E3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19E9E8D9-681F-43BD-BAB6-003827294E0B}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{FA12262A-488B-4907-8A1D-562E1E59E3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27341DDD-5B42-4D6B-979E-53B13B75A187}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E665A9BF-51E9-4189-A511-D13769FDC394}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Taul1!$A$1:$U$48</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -95,33 +98,6 @@
     <t>24.2.</t>
   </si>
   <si>
-    <t>3000-3999</t>
-  </si>
-  <si>
-    <t>2000-2999</t>
-  </si>
-  <si>
-    <t>1000-1999</t>
-  </si>
-  <si>
-    <t>8000-8999</t>
-  </si>
-  <si>
-    <t>9000-9999</t>
-  </si>
-  <si>
-    <t>4000-4999</t>
-  </si>
-  <si>
-    <t>10000-10999</t>
-  </si>
-  <si>
-    <t>13000-13999</t>
-  </si>
-  <si>
-    <t>0-999</t>
-  </si>
-  <si>
     <t>X_luokka</t>
   </si>
   <si>
@@ -138,6 +114,33 @@
   </si>
   <si>
     <t>Y_KA_ero</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1000-1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2000-2999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3000-3999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4000-4999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8000-8999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9000-9999</t>
+  </si>
+  <si>
+    <t>13000-13999</t>
+  </si>
+  <si>
+    <t>10000-10999</t>
   </si>
 </sst>
 </file>
@@ -497,12 +500,13 @@
   <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S42" sqref="S42"/>
+      <selection activeCell="U2" sqref="A2:U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="6" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
     <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" customWidth="1"/>
     <col min="21" max="21" width="14.85546875" customWidth="1"/>
@@ -555,22 +559,22 @@
         <v>17</v>
       </c>
       <c r="P1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -642,10 +646,10 @@
         <v>-1</v>
       </c>
       <c r="T2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="U2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -717,10 +721,10 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -792,10 +796,10 @@
         <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -867,10 +871,10 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -942,10 +946,10 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1017,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="T7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1092,10 +1096,10 @@
         <v>2</v>
       </c>
       <c r="T8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1167,10 +1171,10 @@
         <v>1.5</v>
       </c>
       <c r="T9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="U9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1242,10 +1246,10 @@
         <v>-1.5</v>
       </c>
       <c r="T10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1317,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="T11" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1392,10 +1396,10 @@
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="U12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1467,10 +1471,10 @@
         <v>2</v>
       </c>
       <c r="T13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="U13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1542,10 +1546,10 @@
         <v>2</v>
       </c>
       <c r="T14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1617,10 +1621,10 @@
         <v>1</v>
       </c>
       <c r="T15" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U15" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1692,10 +1696,10 @@
         <v>2</v>
       </c>
       <c r="T16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="U16" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1767,10 +1771,10 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="U17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1842,10 +1846,10 @@
         <v>2</v>
       </c>
       <c r="T18" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U18" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1917,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="T19" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1992,10 +1996,10 @@
         <v>2</v>
       </c>
       <c r="T20" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="U20" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2067,10 +2071,10 @@
         <v>1.5</v>
       </c>
       <c r="T21" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="U21" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2142,10 +2146,10 @@
         <v>2</v>
       </c>
       <c r="T22" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U22" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2217,10 +2221,10 @@
         <v>1</v>
       </c>
       <c r="T23" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U23" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2292,10 +2296,10 @@
         <v>1</v>
       </c>
       <c r="T24" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U24" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2367,10 +2371,10 @@
         <v>2</v>
       </c>
       <c r="T25" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U25" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -2442,10 +2446,10 @@
         <v>2</v>
       </c>
       <c r="T26" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U26" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2517,10 +2521,10 @@
         <v>2</v>
       </c>
       <c r="T27" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U27" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -2592,10 +2596,10 @@
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U28" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -2667,10 +2671,10 @@
         <v>1</v>
       </c>
       <c r="T29" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U29" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -2742,10 +2746,10 @@
         <v>1</v>
       </c>
       <c r="T30" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U30" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -2817,10 +2821,10 @@
         <v>1</v>
       </c>
       <c r="T31" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U31" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -2892,10 +2896,10 @@
         <v>1.5</v>
       </c>
       <c r="T32" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U32" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -2967,10 +2971,10 @@
         <v>2</v>
       </c>
       <c r="T33" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3042,10 +3046,10 @@
         <v>2</v>
       </c>
       <c r="T34" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="U34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -3117,10 +3121,10 @@
         <v>1.5</v>
       </c>
       <c r="T35" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U35" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3192,10 +3196,10 @@
         <v>1</v>
       </c>
       <c r="T36" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="U36" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3267,10 +3271,10 @@
         <v>0</v>
       </c>
       <c r="T37" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="U37" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3342,10 +3346,10 @@
         <v>1</v>
       </c>
       <c r="T38" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="U38" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -3417,10 +3421,10 @@
         <v>1</v>
       </c>
       <c r="T39" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U39" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -3492,10 +3496,10 @@
         <v>1</v>
       </c>
       <c r="T40" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U40" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -3567,10 +3571,10 @@
         <v>1</v>
       </c>
       <c r="T41" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U41" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -3642,10 +3646,10 @@
         <v>1</v>
       </c>
       <c r="T42" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U42" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -3717,10 +3721,10 @@
         <v>1.5</v>
       </c>
       <c r="T43" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="U43" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -3792,10 +3796,10 @@
         <v>1</v>
       </c>
       <c r="T44" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U44" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -3867,10 +3871,10 @@
         <v>2</v>
       </c>
       <c r="T45" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="U45" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -3942,10 +3946,10 @@
         <v>1</v>
       </c>
       <c r="T46" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U46" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -4017,10 +4021,10 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U47" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -4092,13 +4096,14 @@
         <v>0</v>
       </c>
       <c r="T48" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U48" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U48" xr:uid="{2CC713A3-E190-46F0-AA40-E0BFB9B4240C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>